<commit_message>
Output datasheet updated with experiments detail
</commit_message>
<xml_diff>
--- a/Project/Output of Dataset with variable HTM Parameters.xlsx
+++ b/Project/Output of Dataset with variable HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CF8C44-1B30-40D3-8DFD-2C040EBC1F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F31FC10-81AA-453B-A088-2D444BF946DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
   <si>
     <t>S.No</t>
   </si>
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,8 +756,12 @@
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.25</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>17</v>
       </c>
@@ -771,6 +775,35 @@
         <v>21</v>
       </c>
       <c r="I11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Output result file updated
</commit_message>
<xml_diff>
--- a/Project/Output of Dataset with variable HTM Parameters.xlsx
+++ b/Project/Output of Dataset with variable HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F31FC10-81AA-453B-A088-2D444BF946DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB54AF1-05E2-49E2-B857-8459D19BDDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>S.No</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>100*100</t>
+  </si>
+  <si>
+    <t>Test Exp 11</t>
+  </si>
+  <si>
+    <t>Test Exp 12</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,7 +789,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2">
         <v>30</v>
@@ -804,6 +810,35 @@
         <v>21</v>
       </c>
       <c r="I12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Output File details updated
</commit_message>
<xml_diff>
--- a/Project/Output of Dataset with variable HTM Parameters.xlsx
+++ b/Project/Output of Dataset with variable HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB54AF1-05E2-49E2-B857-8459D19BDDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F448886-1173-4F9B-8B9B-FB2435CABB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
   <si>
     <t>S.No</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Test Exp 12</t>
+  </si>
+  <si>
+    <t>Test Exp 13</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,6 +845,35 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating the sheet with experiments detail
</commit_message>
<xml_diff>
--- a/Project/Output of Dataset with variable HTM Parameters.xlsx
+++ b/Project/Output of Dataset with variable HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C628491-7607-4476-B54F-30F3D34ADD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EBD409-BA39-462E-9C94-8F25C35DCE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
   <si>
     <t>S.No</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Test Exp 14</t>
+  </si>
+  <si>
+    <t>Test Exp 15</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,6 +909,35 @@
         <v>26</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
updated the prediction code and output folders
</commit_message>
<xml_diff>
--- a/Project/Output of Dataset with variable HTM Parameters.xlsx
+++ b/Project/Output of Dataset with variable HTM Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0D1F44-E4AB-4CD9-82D1-E0DBFEBB0CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC077EE-0A3E-49E1-9F9B-495E8B8DE4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
   <si>
     <t>S.No</t>
   </si>
@@ -130,6 +130,24 @@
   </si>
   <si>
     <t>Test Exp 17</t>
+  </si>
+  <si>
+    <t>Test Exp 18</t>
+  </si>
+  <si>
+    <t>Test Exp 19</t>
+  </si>
+  <si>
+    <t>Test Exp 20</t>
+  </si>
+  <si>
+    <t>Test Exp 21</t>
+  </si>
+  <si>
+    <t>Test Exp 22</t>
+  </si>
+  <si>
+    <t>Test Exp 23</t>
   </si>
 </sst>
 </file>
@@ -153,15 +171,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -169,18 +199,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +532,7 @@
     <col min="6" max="6" width="31.21875" customWidth="1"/>
     <col min="7" max="7" width="15.77734375" customWidth="1"/>
     <col min="8" max="8" width="17.5546875" customWidth="1"/>
-    <col min="9" max="9" width="28.5546875" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -534,7 +589,7 @@
       <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -563,7 +618,7 @@
       <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -592,7 +647,7 @@
       <c r="H4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -621,7 +676,7 @@
       <c r="H5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -650,7 +705,7 @@
       <c r="H6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -679,7 +734,7 @@
       <c r="H7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -708,7 +763,7 @@
       <c r="H8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -737,7 +792,7 @@
       <c r="H9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -766,7 +821,7 @@
       <c r="H10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -795,7 +850,7 @@
       <c r="H11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -824,7 +879,7 @@
       <c r="H12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -853,7 +908,7 @@
       <c r="H13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -882,7 +937,7 @@
       <c r="H14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -911,7 +966,7 @@
       <c r="H15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -940,7 +995,7 @@
       <c r="H16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -969,7 +1024,7 @@
       <c r="H17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -998,7 +1053,210 @@
       <c r="H18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="2">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="4">
+        <v>30</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="7">
+        <v>30</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="7">
+        <v>30</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="7">
+        <v>30</v>
+      </c>
+      <c r="D23" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="7">
+        <v>30</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="7">
+        <v>30</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Documentation of the project
</commit_message>
<xml_diff>
--- a/Project/Output of Dataset with variable HTM Parameters.xlsx
+++ b/Project/Output of Dataset with variable HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC077EE-0A3E-49E1-9F9B-495E8B8DE4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DED658D-C9D3-4A88-B6D3-A2DBBC9F5A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="74">
   <si>
     <t>S.No</t>
   </si>
@@ -148,13 +148,112 @@
   </si>
   <si>
     <t>Test Exp 23</t>
+  </si>
+  <si>
+    <t>0,1,9</t>
+  </si>
+  <si>
+    <t>Link to the result Output</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%201/Experiment%201%20Image%20classification%20code%20test.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%202/Experiment%20Test%202%20result%20with%20MNIST%20dataset%20of%200%2C1%2C2%20images.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%203/Exp3%20output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%204/Output%20with%20changes%20in%20JSON%20file.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%205/Ouput%20Image%201.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%206/Output%20Image%202.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%207/Output%20Image%207.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%208/Output%20Image%201.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%209/Output%209.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2010/Output%2010.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2011/Output%2010.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2012/output%2012.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2013/output%2013.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2014/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2015/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2016/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2017/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2018/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2019/Output.JPG</t>
+  </si>
+  <si>
+    <t>Test Exp 24</t>
+  </si>
+  <si>
+    <t>Test Exp 25</t>
+  </si>
+  <si>
+    <t>Test Exp 26</t>
+  </si>
+  <si>
+    <t>Test Exp 27</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2020/output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2021/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2022/output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2023/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2024/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2025/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2026/Output.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2027/Output.JPG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +269,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,12 +288,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,10 +316,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -232,12 +334,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -516,26 +620,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" customWidth="1"/>
-    <col min="6" max="6" width="31.21875" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="20.21875" customWidth="1"/>
+    <col min="10" max="10" width="174.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,8 +667,11 @@
       <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -592,8 +699,11 @@
       <c r="I2" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -621,8 +731,11 @@
       <c r="I3" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -650,8 +763,11 @@
       <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -679,8 +795,11 @@
       <c r="I5" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -708,8 +827,11 @@
       <c r="I6" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -737,8 +859,11 @@
       <c r="I7" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -766,8 +891,11 @@
       <c r="I8" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -795,8 +923,11 @@
       <c r="I9" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -824,8 +955,11 @@
       <c r="I10" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -853,8 +987,11 @@
       <c r="I11" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -882,8 +1019,11 @@
       <c r="I12" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -911,8 +1051,11 @@
       <c r="I13" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -940,8 +1083,11 @@
       <c r="I14" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -969,8 +1115,11 @@
       <c r="I15" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -998,8 +1147,11 @@
       <c r="I16" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1027,8 +1179,11 @@
       <c r="I17" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1056,8 +1211,11 @@
       <c r="I18" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1085,8 +1243,11 @@
       <c r="I19" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1114,154 +1275,296 @@
       <c r="I20" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
+      <c r="J20" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="7">
-        <v>30</v>
-      </c>
-      <c r="D21" s="7">
+      <c r="C21" s="4">
+        <v>10</v>
+      </c>
+      <c r="D21" s="4">
         <v>0.75</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="7" t="s">
+      <c r="E21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>21</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="7">
-        <v>30</v>
-      </c>
-      <c r="D22" s="7">
+      <c r="I21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="4">
+        <v>10</v>
+      </c>
+      <c r="D22" s="4">
         <v>0.8</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="7" t="s">
+      <c r="E22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+      <c r="I22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="7">
-        <v>30</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="B23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="4">
+        <v>10</v>
+      </c>
+      <c r="D23" s="4">
         <v>0.85</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="7" t="s">
+      <c r="E23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
+      <c r="I23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="7">
-        <v>30</v>
-      </c>
-      <c r="D24" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="7" t="s">
+      <c r="B24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="4">
+        <v>10</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
+      <c r="I24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="7">
-        <v>30</v>
-      </c>
-      <c r="D25" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="7" t="s">
+      <c r="B25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="4">
+        <v>10</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>26</v>
+      <c r="I25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="4">
+        <v>10</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="4">
+        <v>10</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="4">
+        <v>10</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{5C1A984F-28BF-4554-A4AC-E9A4CA538F48}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{A1B9FFFF-3CE7-4EA8-B3A8-73E8E2196683}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{79462FA7-368E-45B6-AA51-6213FDA940B0}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{EAA25E8A-AF14-4917-BC66-557BD367769C}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{67BDAB6D-9944-4CBE-93A5-957992882C20}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{E77CD32A-FAC1-40F1-B5A3-BAE73F0328BB}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{B6DAB0D2-E268-467F-B3F9-817C30663BF5}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{23B4C3E1-45E8-4153-A794-388608F3F52B}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{8C7C0C32-1E8E-425F-94A6-4976B43D75C4}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{F80A18D5-A18D-43B1-B870-2571C9F3F1A7}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{812D2036-25E8-4428-B802-BDA34580E0DA}"/>
+    <hyperlink ref="J14" r:id="rId12" xr:uid="{97948D49-CA06-49FF-A6C9-8588F9890870}"/>
+    <hyperlink ref="J15" r:id="rId13" xr:uid="{95057CC9-6CE7-467E-BA6D-8E809092C716}"/>
+    <hyperlink ref="J16" r:id="rId14" xr:uid="{FDE3F098-98A8-49F3-8CF4-AF56DC6558C7}"/>
+    <hyperlink ref="J17" r:id="rId15" xr:uid="{960092EF-36FA-46C6-B8A3-C18F63913ADA}"/>
+    <hyperlink ref="J18" r:id="rId16" xr:uid="{2DB48C16-7929-4FB4-9BF0-8306971A42FA}"/>
+    <hyperlink ref="J19" r:id="rId17" xr:uid="{999C63AF-2BB8-4FCB-9400-4B2E5030EC71}"/>
+    <hyperlink ref="J20" r:id="rId18" xr:uid="{65E99FA1-EF9A-4032-AE3C-1EED71A28B2D}"/>
+    <hyperlink ref="J21" r:id="rId19" xr:uid="{529E51F4-B3F5-4015-B0A7-56FE217821F5}"/>
+    <hyperlink ref="J22" r:id="rId20" xr:uid="{5FC0339D-C5EB-4C61-ABDB-C810EEA03B60}"/>
+    <hyperlink ref="J23" r:id="rId21" xr:uid="{2B1ADE86-13AC-468D-AFD8-3047255A37F7}"/>
+    <hyperlink ref="J24" r:id="rId22" xr:uid="{7EDA95A7-A7D6-4D26-8DF7-4BEAD022C9F4}"/>
+    <hyperlink ref="J25" r:id="rId23" xr:uid="{3F11A10B-3B61-44F1-A02F-0CF1AA63C332}"/>
+    <hyperlink ref="J26" r:id="rId24" xr:uid="{7B104721-69BC-4289-A025-77D2C07472AB}"/>
+    <hyperlink ref="J27" r:id="rId25" xr:uid="{A0EF5416-3769-41FB-BFA7-2A3856B9C3DA}"/>
+    <hyperlink ref="J28" r:id="rId26" xr:uid="{6287B25D-5078-4D86-9527-E1C2476B3EE9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>